<commit_message>
Modified Schema Excel and Added Activity_Board_System Docx Files
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\ITECC05\MAINPRX\PRX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389D0603-514C-40BD-A349-877AE328D31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3DDA1E-67E9-4650-A4E4-A41D441F02BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="113">
   <si>
     <t>db_reminder</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>/api/superadmin/changePrivillege</t>
-  </si>
-  <si>
     <t>Member</t>
   </si>
   <si>
@@ -214,18 +211,12 @@
     <t>createRequest</t>
   </si>
   <si>
-    <t>deleteRequest</t>
-  </si>
-  <si>
     <t>/api/requests</t>
   </si>
   <si>
     <t>/api/requests/create</t>
   </si>
   <si>
-    <t>/api/requests/delete</t>
-  </si>
-  <si>
     <t>requestsModel</t>
   </si>
   <si>
@@ -304,9 +295,6 @@
     <t>getRequestsByStatus</t>
   </si>
   <si>
-    <t>/api/user</t>
-  </si>
-  <si>
     <t>getCurrentUser</t>
   </si>
   <si>
@@ -328,9 +316,6 @@
     <t>/api/admin/activites/delete/:id</t>
   </si>
   <si>
-    <t>/api/admin/requests/status</t>
-  </si>
-  <si>
     <t>Methods</t>
   </si>
   <si>
@@ -365,6 +350,15 @@
   </si>
   <si>
     <t>Special Attributes</t>
+  </si>
+  <si>
+    <t>/api/user/:id</t>
+  </si>
+  <si>
+    <t>/api/superadmin/changePrivillege/:id</t>
+  </si>
+  <si>
+    <t>/api/admin/requests/status/:id</t>
   </si>
 </sst>
 </file>
@@ -480,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -493,8 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -848,7 +840,7 @@
     <col min="5" max="5" width="31.75" customWidth="1"/>
     <col min="6" max="6" width="25.83203125" customWidth="1"/>
     <col min="7" max="7" width="27.83203125" customWidth="1"/>
-    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="8" max="8" width="34.1640625" customWidth="1"/>
     <col min="9" max="9" width="28.08203125" customWidth="1"/>
     <col min="10" max="10" width="28.9140625" customWidth="1"/>
     <col min="11" max="11" width="28.08203125" customWidth="1"/>
@@ -881,7 +873,7 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -892,7 +884,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -916,7 +908,7 @@
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M4" t="s">
         <v>20</v>
@@ -933,7 +925,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -957,7 +949,7 @@
         <v>10</v>
       </c>
       <c r="L5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M5" t="s">
         <v>26</v>
@@ -974,31 +966,31 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" t="s">
         <v>94</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" t="s">
         <v>96</v>
       </c>
-      <c r="F6" t="s">
+      <c r="K6" t="s">
         <v>97</v>
       </c>
-      <c r="G6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" t="s">
-        <v>99</v>
-      </c>
-      <c r="J6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K6" t="s">
-        <v>101</v>
-      </c>
       <c r="L6" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="M6" t="s">
         <v>30</v>
@@ -1042,7 +1034,7 @@
         <v>14</v>
       </c>
       <c r="M7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1061,7 +1053,7 @@
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1070,9 +1062,9 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="9">
@@ -1081,9 +1073,9 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -1092,48 +1084,44 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
-      <c r="C13" s="10"/>
       <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
-      <c r="C14" s="10"/>
       <c r="D14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
-      <c r="C16" s="10"/>
       <c r="D16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
-      <c r="C17" s="10"/>
       <c r="D17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -1142,9 +1130,9 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -1153,9 +1141,9 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -1164,94 +1152,94 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="D21" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" t="s">
         <v>43</v>
       </c>
-      <c r="C25" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>44</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>45</v>
-      </c>
-      <c r="F25" t="s">
-        <v>46</v>
       </c>
       <c r="G25" t="s">
         <v>20</v>
       </c>
       <c r="H25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" t="s">
         <v>43</v>
       </c>
-      <c r="C26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>44</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>45</v>
-      </c>
-      <c r="F26" t="s">
-        <v>46</v>
       </c>
       <c r="G26" t="s">
         <v>26</v>
       </c>
       <c r="H26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F27" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G27" t="s">
         <v>30</v>
       </c>
       <c r="H27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1271,7 +1259,7 @@
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1289,7 +1277,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B31" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
         <v>24</v>
@@ -1301,200 +1289,191 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B32" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
         <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
       <c r="D34" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B35" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B36" s="4"/>
       <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
         <v>54</v>
-      </c>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B37" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" t="s">
-        <v>55</v>
       </c>
       <c r="D37" t="s">
         <v>25</v>
       </c>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B38" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
         <v>25</v>
       </c>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B39" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
         <v>24</v>
       </c>
       <c r="D39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B40" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B40" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" t="s">
-        <v>57</v>
-      </c>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B41" s="4"/>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B42" s="4"/>
       <c r="D42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="8"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" t="s">
+        <v>107</v>
+      </c>
+      <c r="E46" t="s">
         <v>62</v>
       </c>
-      <c r="C46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" t="s">
-        <v>112</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+      <c r="G47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
         <v>63</v>
       </c>
-      <c r="F46" t="s">
+      <c r="C48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48" t="s">
         <v>64</v>
       </c>
-      <c r="G46" t="s">
-        <v>20</v>
-      </c>
-      <c r="H46" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47" t="s">
-        <v>112</v>
-      </c>
-      <c r="E47" t="s">
-        <v>63</v>
-      </c>
-      <c r="F47" t="s">
-        <v>64</v>
-      </c>
-      <c r="G47" t="s">
-        <v>26</v>
-      </c>
-      <c r="H47" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" t="s">
-        <v>111</v>
-      </c>
-      <c r="D48" t="s">
-        <v>113</v>
-      </c>
-      <c r="E48" t="s">
-        <v>66</v>
-      </c>
       <c r="F48" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" t="s">
         <v>67</v>
       </c>
-      <c r="G48" t="s">
-        <v>30</v>
-      </c>
-      <c r="H48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>14</v>
       </c>
@@ -1508,14 +1487,11 @@
         <v>13</v>
       </c>
       <c r="F49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
         <v>17</v>
       </c>
@@ -1527,157 +1503,153 @@
       </c>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B52" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B53" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B54" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B55" s="4"/>
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B56" s="4"/>
+      <c r="D56" t="s">
+        <v>104</v>
+      </c>
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B57" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B58" s="4"/>
+      <c r="D58" t="s">
+        <v>53</v>
+      </c>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B59" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B60" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B61" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" t="s">
+        <v>54</v>
+      </c>
+      <c r="D61" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B62" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" t="s">
+        <v>55</v>
+      </c>
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B63" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B53" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B54" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B55" s="4"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B56" s="4"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E56" s="5"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B57" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E57" s="5"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B58" s="4"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B59" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B60" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B61" s="4" t="s">
+      <c r="C63" t="s">
+        <v>24</v>
+      </c>
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B64" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E61" s="5"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B62" s="4" t="s">
+      <c r="C64" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" t="s">
         <v>87</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B63" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B64" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="E64" s="5"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B65" s="4"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10" t="s">
-        <v>91</v>
+      <c r="D65" t="s">
+        <v>88</v>
       </c>
       <c r="E65" s="5"/>
     </row>
@@ -1685,15 +1657,9 @@
       <c r="B66" s="6"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E66" s="8"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the word and excel files
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\ITECC05\MAINPRX\PRX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3DDA1E-67E9-4650-A4E4-A41D441F02BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6725ED66-895D-4E8F-AC29-0654E7B5E889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
   <si>
     <t>db_reminder</t>
   </si>
@@ -256,12 +256,6 @@
     <t>activityDeadline</t>
   </si>
   <si>
-    <t>activityCreated</t>
-  </si>
-  <si>
-    <t>activityCreator</t>
-  </si>
-  <si>
     <t>activityStatus</t>
   </si>
   <si>
@@ -271,12 +265,6 @@
     <t>requestHeader</t>
   </si>
   <si>
-    <t>requestCreated</t>
-  </si>
-  <si>
-    <t>requestCreator</t>
-  </si>
-  <si>
     <t>requestDescription</t>
   </si>
   <si>
@@ -359,6 +347,24 @@
   </si>
   <si>
     <t>/api/admin/requests/status/:id</t>
+  </si>
+  <si>
+    <t>activityPublished</t>
+  </si>
+  <si>
+    <t>requestPublished</t>
+  </si>
+  <si>
+    <t>requestPublisher</t>
+  </si>
+  <si>
+    <t>activityPublisher</t>
+  </si>
+  <si>
+    <t>getRequestsByDatePublished</t>
+  </si>
+  <si>
+    <t>/api/requests/date_published/:date</t>
   </si>
 </sst>
 </file>
@@ -474,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -485,6 +491,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -828,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46:G49"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -873,7 +882,7 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -884,7 +893,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -908,7 +917,7 @@
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M4" t="s">
         <v>20</v>
@@ -925,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -949,7 +958,7 @@
         <v>10</v>
       </c>
       <c r="L5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M5" t="s">
         <v>26</v>
@@ -966,31 +975,31 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" t="s">
         <v>92</v>
       </c>
-      <c r="F6" t="s">
+      <c r="K6" t="s">
         <v>93</v>
       </c>
-      <c r="G6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H6" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" t="s">
-        <v>97</v>
-      </c>
       <c r="L6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="M6" t="s">
         <v>30</v>
@@ -1034,7 +1043,7 @@
         <v>14</v>
       </c>
       <c r="M7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1178,7 +1187,7 @@
         <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
         <v>43</v>
@@ -1201,7 +1210,7 @@
         <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s">
         <v>43</v>
@@ -1224,16 +1233,16 @@
         <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G27" t="s">
         <v>30</v>
@@ -1259,7 +1268,7 @@
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1298,24 +1307,24 @@
         <v>49</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="D33" t="s">
         <v>51</v>
       </c>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B35" s="4" t="s">
         <v>76</v>
       </c>
@@ -1327,40 +1336,35 @@
       </c>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B36" s="4"/>
       <c r="D36" t="s">
         <v>53</v>
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B37" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
       </c>
-      <c r="D37" t="s">
-        <v>25</v>
-      </c>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B38" s="4" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
         <v>54</v>
       </c>
-      <c r="D38" t="s">
-        <v>25</v>
-      </c>
+      <c r="D38" s="10"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B39" s="4" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
         <v>24</v>
@@ -1370,9 +1374,9 @@
       </c>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B40" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
         <v>24</v>
@@ -1382,23 +1386,23 @@
       </c>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B41" s="4"/>
       <c r="D41" t="s">
         <v>57</v>
       </c>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B42" s="4"/>
       <c r="D42" t="s">
         <v>58</v>
       </c>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>24</v>
@@ -1408,72 +1412,81 @@
       </c>
       <c r="E43" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D46" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E46" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" t="s">
         <v>62</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>20</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>61</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E47" t="s">
+        <v>113</v>
+      </c>
+      <c r="F47" t="s">
         <v>62</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>26</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E48" t="s">
+        <v>114</v>
+      </c>
+      <c r="F48" t="s">
         <v>64</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>30</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>14</v>
       </c>
@@ -1484,14 +1497,17 @@
         <v>14</v>
       </c>
       <c r="E49" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" t="s">
         <v>13</v>
       </c>
-      <c r="F49" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
         <v>17</v>
       </c>
@@ -1503,9 +1519,9 @@
       </c>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C52" t="s">
         <v>24</v>
@@ -1515,7 +1531,7 @@
       </c>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B53" s="4" t="s">
         <v>74</v>
       </c>
@@ -1527,7 +1543,7 @@
       </c>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B54" s="4" t="s">
         <v>75</v>
       </c>
@@ -1538,24 +1554,24 @@
         <v>49</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B55" s="4"/>
       <c r="D55" t="s">
         <v>51</v>
       </c>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B56" s="4"/>
       <c r="D56" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B57" s="4" t="s">
         <v>76</v>
       </c>
@@ -1567,28 +1583,25 @@
       </c>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B58" s="4"/>
       <c r="D58" t="s">
         <v>53</v>
       </c>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B59" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C59" t="s">
         <v>54</v>
       </c>
-      <c r="D59" t="s">
-        <v>25</v>
-      </c>
       <c r="E59" s="5"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B60" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
         <v>24</v>
@@ -1598,21 +1611,18 @@
       </c>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B61" s="4" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="C61" t="s">
         <v>54</v>
       </c>
-      <c r="D61" t="s">
-        <v>25</v>
-      </c>
       <c r="E61" s="5"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B62" s="4" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="C62" t="s">
         <v>24</v>
@@ -1622,9 +1632,9 @@
       </c>
       <c r="E62" s="5"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B63" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C63" t="s">
         <v>24</v>
@@ -1634,22 +1644,22 @@
       </c>
       <c r="E63" s="5"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B64" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C64" t="s">
         <v>24</v>
       </c>
       <c r="D64" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E64" s="5"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B65" s="4"/>
       <c r="D65" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E65" s="5"/>
     </row>
@@ -1657,14 +1667,14 @@
       <c r="B66" s="6"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E66" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:M2 E14:M14 A11:A22 E19:M19 K25:K28 E12:G13 E15:F18 E21:M22 E20:K20 M20 A8:M8 A3:G3 A1:L1 A4:C7 K15:M18 A9:D10 I9:M13 G9:G11 M23:M24 M29:M62" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:M2 E14:M14 A11:A22 E19:M19 K25:K28 E12:G13 E15:F18 E21:M22 E20:K20 M20 A8:M8 A3:G3 A1:L1 A5:C7 K15:M18 A9:D10 I9:M13 G9:G11 M23:M24 M29:M62 A4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified few excel tables
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\ITECC05\PRX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F27C828-F052-4B8A-B2CC-6067F612905B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF619E6A-FA2D-44C0-91A0-E798B74F41C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="127">
   <si>
     <t>db_reminder</t>
   </si>
@@ -238,15 +238,6 @@
     <t>activityStatus</t>
   </si>
   <si>
-    <t>upcoming</t>
-  </si>
-  <si>
-    <t>concluded</t>
-  </si>
-  <si>
-    <t>canceled</t>
-  </si>
-  <si>
     <t>activityDescription</t>
   </si>
   <si>
@@ -398,6 +389,18 @@
   </si>
   <si>
     <t>/abs/requests/datePublished/:date</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>Concluded</t>
+  </si>
+  <si>
+    <t>Canceled</t>
+  </si>
+  <si>
+    <t>Subject (ex. Science, Math)</t>
   </si>
 </sst>
 </file>
@@ -776,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -828,25 +831,25 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
         <v>108</v>
       </c>
-      <c r="G4" t="s">
-        <v>111</v>
-      </c>
       <c r="H4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -855,7 +858,7 @@
         <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>
@@ -867,7 +870,7 @@
         <v>15</v>
       </c>
       <c r="O4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P4" t="s">
         <v>16</v>
@@ -884,13 +887,13 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -905,7 +908,7 @@
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L5" t="s">
         <v>12</v>
@@ -917,7 +920,7 @@
         <v>15</v>
       </c>
       <c r="O5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P5" t="s">
         <v>18</v>
@@ -928,46 +931,46 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" t="s">
         <v>101</v>
       </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" t="s">
-        <v>104</v>
-      </c>
       <c r="J6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="P6" t="s">
         <v>20</v>
@@ -1025,7 +1028,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -1205,19 +1208,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
         <v>92</v>
       </c>
-      <c r="C27" t="s">
+      <c r="F27" t="s">
         <v>93</v>
-      </c>
-      <c r="D27" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" t="s">
-        <v>96</v>
       </c>
       <c r="G27" t="s">
         <v>20</v>
@@ -1315,6 +1318,9 @@
       <c r="C37" t="s">
         <v>67</v>
       </c>
+      <c r="D37" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
@@ -1323,6 +1329,9 @@
       <c r="C38" t="s">
         <v>67</v>
       </c>
+      <c r="D38" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
@@ -1343,102 +1352,102 @@
         <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D41" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
         <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F46" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G46" t="s">
         <v>16</v>
       </c>
       <c r="H46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E47" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F47" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G47" t="s">
         <v>18</v>
       </c>
       <c r="H47" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" t="s">
         <v>97</v>
-      </c>
-      <c r="C48" t="s">
-        <v>98</v>
-      </c>
-      <c r="D48" t="s">
-        <v>99</v>
-      </c>
-      <c r="E48" t="s">
-        <v>125</v>
-      </c>
-      <c r="F48" t="s">
-        <v>100</v>
       </c>
       <c r="G48" t="s">
         <v>20</v>
       </c>
       <c r="H48" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.35">
@@ -1474,7 +1483,7 @@
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
         <v>31</v>
@@ -1531,7 +1540,7 @@
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D58" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.35">
@@ -1541,29 +1550,35 @@
       <c r="C59" t="s">
         <v>67</v>
       </c>
+      <c r="D59" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
         <v>31</v>
       </c>
       <c r="D60" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s">
         <v>67</v>
       </c>
+      <c r="D61" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
         <v>31</v>
@@ -1574,40 +1589,40 @@
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
         <v>31</v>
       </c>
       <c r="D63" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C64" t="s">
         <v>31</v>
       </c>
       <c r="D64" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D65" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D66" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:O2 A26:O26 A25:C25 G25:O25 A9:O11 A6 A28:O45 A27 G27:O27 A49:O66 A48 G48:O48 A14:O20 A12:E12 G12:O12 A13:E13 G13:O13 A3:C3 A7:C7 A5:B5 A4 A8:B8 D8:O8 A22:O24 A21:B21 D21:O21 A47:D47 A46:D46 F46:O46 F47:O47" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:O2 A26:O26 A25:C25 G25:O25 A9:O11 A6 A28:O36 A27 G27:O27 A49:O56 A48 G48:O48 A14:O20 A12:E12 G12:O12 A13:E13 G13:O13 A3:C3 A7:C7 A5:B5 A4 A8:B8 D8:O8 A22:O24 A21:B21 D21:O21 A47:D47 A46:D46 F46:O46 F47:O47 A60:O60 A59:C59 E59:O59 A62:O66 A61:C61 E61:O61 A43:O45 A37:C37 E37:O37 A38:C38 E38:O38 A39:C39 E39:O39 A40:C40 E40:O40 A41:C41 E41:O41 A42:C42 E42:O42 A58:C58 A57:C57 E57:O57 E58:O58" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Excel Tables (#55)
* Added a feature where Approved requests gets added to the activities table

* Modified few excel tables
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\ITECC05\PRX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F27C828-F052-4B8A-B2CC-6067F612905B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF619E6A-FA2D-44C0-91A0-E798B74F41C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="127">
   <si>
     <t>db_reminder</t>
   </si>
@@ -238,15 +238,6 @@
     <t>activityStatus</t>
   </si>
   <si>
-    <t>upcoming</t>
-  </si>
-  <si>
-    <t>concluded</t>
-  </si>
-  <si>
-    <t>canceled</t>
-  </si>
-  <si>
     <t>activityDescription</t>
   </si>
   <si>
@@ -398,6 +389,18 @@
   </si>
   <si>
     <t>/abs/requests/datePublished/:date</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>Concluded</t>
+  </si>
+  <si>
+    <t>Canceled</t>
+  </si>
+  <si>
+    <t>Subject (ex. Science, Math)</t>
   </si>
 </sst>
 </file>
@@ -776,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -828,25 +831,25 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
         <v>108</v>
       </c>
-      <c r="G4" t="s">
-        <v>111</v>
-      </c>
       <c r="H4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -855,7 +858,7 @@
         <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>
@@ -867,7 +870,7 @@
         <v>15</v>
       </c>
       <c r="O4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P4" t="s">
         <v>16</v>
@@ -884,13 +887,13 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -905,7 +908,7 @@
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L5" t="s">
         <v>12</v>
@@ -917,7 +920,7 @@
         <v>15</v>
       </c>
       <c r="O5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P5" t="s">
         <v>18</v>
@@ -928,46 +931,46 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" t="s">
         <v>101</v>
       </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" t="s">
-        <v>104</v>
-      </c>
       <c r="J6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="P6" t="s">
         <v>20</v>
@@ -1025,7 +1028,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -1205,19 +1208,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
         <v>92</v>
       </c>
-      <c r="C27" t="s">
+      <c r="F27" t="s">
         <v>93</v>
-      </c>
-      <c r="D27" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" t="s">
-        <v>96</v>
       </c>
       <c r="G27" t="s">
         <v>20</v>
@@ -1315,6 +1318,9 @@
       <c r="C37" t="s">
         <v>67</v>
       </c>
+      <c r="D37" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
@@ -1323,6 +1329,9 @@
       <c r="C38" t="s">
         <v>67</v>
       </c>
+      <c r="D38" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
@@ -1343,102 +1352,102 @@
         <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D41" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
         <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F46" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G46" t="s">
         <v>16</v>
       </c>
       <c r="H46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E47" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F47" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G47" t="s">
         <v>18</v>
       </c>
       <c r="H47" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" t="s">
         <v>97</v>
-      </c>
-      <c r="C48" t="s">
-        <v>98</v>
-      </c>
-      <c r="D48" t="s">
-        <v>99</v>
-      </c>
-      <c r="E48" t="s">
-        <v>125</v>
-      </c>
-      <c r="F48" t="s">
-        <v>100</v>
       </c>
       <c r="G48" t="s">
         <v>20</v>
       </c>
       <c r="H48" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.35">
@@ -1474,7 +1483,7 @@
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
         <v>31</v>
@@ -1531,7 +1540,7 @@
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D58" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.35">
@@ -1541,29 +1550,35 @@
       <c r="C59" t="s">
         <v>67</v>
       </c>
+      <c r="D59" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
         <v>31</v>
       </c>
       <c r="D60" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s">
         <v>67</v>
       </c>
+      <c r="D61" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
         <v>31</v>
@@ -1574,40 +1589,40 @@
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
         <v>31</v>
       </c>
       <c r="D63" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C64" t="s">
         <v>31</v>
       </c>
       <c r="D64" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D65" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D66" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:O2 A26:O26 A25:C25 G25:O25 A9:O11 A6 A28:O45 A27 G27:O27 A49:O66 A48 G48:O48 A14:O20 A12:E12 G12:O12 A13:E13 G13:O13 A3:C3 A7:C7 A5:B5 A4 A8:B8 D8:O8 A22:O24 A21:B21 D21:O21 A47:D47 A46:D46 F46:O46 F47:O47" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:O2 A26:O26 A25:C25 G25:O25 A9:O11 A6 A28:O36 A27 G27:O27 A49:O56 A48 G48:O48 A14:O20 A12:E12 G12:O12 A13:E13 G13:O13 A3:C3 A7:C7 A5:B5 A4 A8:B8 D8:O8 A22:O24 A21:B21 D21:O21 A47:D47 A46:D46 F46:O46 F47:O47 A60:O60 A59:C59 E59:O59 A62:O66 A61:C61 E61:O61 A43:O45 A37:C37 E37:O37 A38:C38 E38:O38 A39:C39 E39:O39 A40:C40 E40:O40 A41:C41 E41:O41 A42:C42 E42:O42 A58:C58 A57:C57 E57:O57 E58:O58" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>